<commit_message>
Added size of DB or HUC12 units
</commit_message>
<xml_diff>
--- a/site_DATAexplore/Landcover_Final.xlsx
+++ b/site_DATAexplore/Landcover_Final.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/williamjohnson/Desktop/Laura/Hallett_Lab/Repositories/thesis-mussels/site_DATAexplore/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB1D47B6-AA04-9947-AC4D-9FD79A16C443}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EBF5ECE-ABD0-3A4B-B4E5-A780016FF7F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="700" yWindow="460" windowWidth="26320" windowHeight="16080" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="47">
   <si>
     <t>site_id</t>
   </si>
@@ -172,6 +172,9 @@
   </si>
   <si>
     <t>ZincCr</t>
+  </si>
+  <si>
+    <t>huc12_area_sq.km</t>
   </si>
 </sst>
 </file>
@@ -1784,10 +1787,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:R11"/>
+  <dimension ref="A1:S11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q9" sqref="Q9"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1795,10 +1798,11 @@
     <col min="1" max="1" width="13.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="47.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="47.33203125" customWidth="1"/>
+    <col min="5" max="5" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -1809,52 +1813,55 @@
         <v>0</v>
       </c>
       <c r="D1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" t="s">
         <v>35</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>34</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>36</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>37</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>38</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>39</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>5</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>43</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>6</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>40</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>7</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>41</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>8</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>171003021305</v>
       </c>
@@ -1864,61 +1871,61 @@
       <c r="C2" t="s">
         <v>29</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>13733</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>24923</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>49766</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>29707</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>33828</v>
       </c>
-      <c r="I2">
+      <c r="J2">
         <v>3205</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>268</v>
       </c>
-      <c r="K2">
-        <f>D2 +E2 +F2 +G2 +H2 +I2 +J2</f>
+      <c r="L2">
+        <f>E2 +F2 +G2 +H2 +I2 +J2 +K2</f>
         <v>155430</v>
       </c>
-      <c r="L2">
-        <f>D2 + E2</f>
+      <c r="M2">
+        <f>E2 + F2</f>
         <v>38656</v>
       </c>
-      <c r="M2">
-        <f>H2/K2 * 100</f>
+      <c r="N2">
+        <f>I2/L2 * 100</f>
         <v>21.764138197259218</v>
       </c>
-      <c r="N2">
-        <f>D2/K2 * 100</f>
+      <c r="O2">
+        <f>E2/L2 * 100</f>
         <v>8.8354886444058423</v>
       </c>
-      <c r="O2">
-        <f>E2/K2 * 100</f>
+      <c r="P2">
+        <f>F2/L2 * 100</f>
         <v>16.03487100302387</v>
       </c>
-      <c r="P2">
-        <f>L2/K2 * 100</f>
+      <c r="Q2">
+        <f>M2/L2 * 100</f>
         <v>24.870359647429709</v>
       </c>
-      <c r="Q2">
-        <f>F2/K2 * 100</f>
+      <c r="R2">
+        <f>G2/L2 * 100</f>
         <v>32.018271890883355</v>
       </c>
-      <c r="R2">
-        <f xml:space="preserve"> G2/K2 * 100</f>
+      <c r="S2">
+        <f xml:space="preserve"> H2/L2 * 100</f>
         <v>19.112783889853954</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>171003021102</v>
       </c>
@@ -1929,60 +1936,63 @@
         <v>12</v>
       </c>
       <c r="D3">
+        <v>215.36</v>
+      </c>
+      <c r="E3">
         <v>5454</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>2503</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>18975</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>49497</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>50495</v>
       </c>
-      <c r="I3">
+      <c r="J3">
         <v>811</v>
       </c>
-      <c r="J3">
+      <c r="K3">
         <v>202</v>
       </c>
-      <c r="K3">
-        <f t="shared" ref="K3:K11" si="0">D3 +E3 +F3 +G3 +H3 +I3 +J3</f>
+      <c r="L3">
+        <f t="shared" ref="L3:L11" si="0">E3 +F3 +G3 +H3 +I3 +J3 +K3</f>
         <v>127937</v>
       </c>
-      <c r="L3">
-        <f t="shared" ref="L3:L11" si="1">D3 + E3</f>
+      <c r="M3">
+        <f t="shared" ref="M3:M11" si="1">E3 + F3</f>
         <v>7957</v>
       </c>
-      <c r="M3">
-        <f t="shared" ref="M3:M11" si="2">H3/K3 * 100</f>
+      <c r="N3">
+        <f t="shared" ref="N3:N11" si="2">I3/L3 * 100</f>
         <v>39.468644723574883</v>
       </c>
-      <c r="N3">
-        <f t="shared" ref="N3:N11" si="3">D3/K3 * 100</f>
+      <c r="O3">
+        <f t="shared" ref="O3:O11" si="3">E3/L3 * 100</f>
         <v>4.2630357128899377</v>
       </c>
-      <c r="O3">
-        <f t="shared" ref="O3:O11" si="4">E3/K3 * 100</f>
+      <c r="P3">
+        <f t="shared" ref="P3:P11" si="4">F3/L3 * 100</f>
         <v>1.9564316812180995</v>
       </c>
-      <c r="P3">
-        <f t="shared" ref="P3:P11" si="5">L3/K3 * 100</f>
+      <c r="Q3">
+        <f t="shared" ref="Q3:Q11" si="5">M3/L3 * 100</f>
         <v>6.2194673941080376</v>
       </c>
-      <c r="Q3">
-        <f t="shared" ref="Q3:Q11" si="6">F3/K3 * 100</f>
+      <c r="R3">
+        <f t="shared" ref="R3:R11" si="6">G3/L3 * 100</f>
         <v>14.831518638079681</v>
       </c>
-      <c r="R3">
-        <f t="shared" ref="R3:R11" si="7" xml:space="preserve"> G3/K3 * 100</f>
+      <c r="S3">
+        <f t="shared" ref="S3:S11" si="7" xml:space="preserve"> H3/L3 * 100</f>
         <v>38.688573282162317</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>171003021101</v>
       </c>
@@ -1993,60 +2003,63 @@
         <v>44</v>
       </c>
       <c r="D4">
+        <v>107.5</v>
+      </c>
+      <c r="E4">
         <v>4523</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>4713</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>10211</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>20565</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>23335</v>
       </c>
-      <c r="I4">
+      <c r="J4">
         <v>489</v>
       </c>
-      <c r="J4">
+      <c r="K4">
         <v>211</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <f t="shared" si="0"/>
         <v>64047</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <f t="shared" si="1"/>
         <v>9236</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <f t="shared" si="2"/>
         <v>36.434181148219274</v>
       </c>
-      <c r="N4">
+      <c r="O4">
         <f t="shared" si="3"/>
         <v>7.0620013427639075</v>
       </c>
-      <c r="O4">
+      <c r="P4">
         <f t="shared" si="4"/>
         <v>7.3586584851749501</v>
       </c>
-      <c r="P4">
+      <c r="Q4">
         <f t="shared" si="5"/>
         <v>14.420659827938859</v>
       </c>
-      <c r="Q4">
+      <c r="R4">
         <f t="shared" si="6"/>
         <v>15.942979374521835</v>
       </c>
-      <c r="R4">
+      <c r="S4">
         <f t="shared" si="7"/>
         <v>32.109232282542507</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>171003020508</v>
       </c>
@@ -2057,60 +2070,63 @@
         <v>17</v>
       </c>
       <c r="D5">
+        <v>200.22</v>
+      </c>
+      <c r="E5">
         <v>3977</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>1886</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>23606</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>26382</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>62931</v>
       </c>
-      <c r="I5">
+      <c r="J5">
         <v>425</v>
       </c>
-      <c r="J5">
+      <c r="K5">
         <v>106</v>
       </c>
-      <c r="K5">
+      <c r="L5">
         <f t="shared" si="0"/>
         <v>119313</v>
       </c>
-      <c r="L5">
+      <c r="M5">
         <f t="shared" si="1"/>
         <v>5863</v>
       </c>
-      <c r="M5">
+      <c r="N5">
         <f t="shared" si="2"/>
         <v>52.74446204520882</v>
       </c>
-      <c r="N5">
+      <c r="O5">
         <f t="shared" si="3"/>
         <v>3.3332495201696379</v>
       </c>
-      <c r="O5">
+      <c r="P5">
         <f t="shared" si="4"/>
         <v>1.5807162672969417</v>
       </c>
-      <c r="P5">
+      <c r="Q5">
         <f t="shared" si="5"/>
         <v>4.9139657874665792</v>
       </c>
-      <c r="Q5">
+      <c r="R5">
         <f t="shared" si="6"/>
         <v>19.784935421957371</v>
       </c>
-      <c r="R5">
+      <c r="S5">
         <f t="shared" si="7"/>
         <v>22.111588846144176</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>171003020506</v>
       </c>
@@ -2121,60 +2137,63 @@
         <v>30</v>
       </c>
       <c r="D6">
+        <v>130.85</v>
+      </c>
+      <c r="E6">
         <v>1124</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>168</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>4683</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>23054</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>48786</v>
       </c>
-      <c r="I6">
+      <c r="J6">
         <v>276</v>
       </c>
-      <c r="J6">
+      <c r="K6">
         <v>86</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <f t="shared" si="0"/>
         <v>78177</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <f t="shared" si="1"/>
         <v>1292</v>
       </c>
-      <c r="M6">
+      <c r="N6">
         <f t="shared" si="2"/>
         <v>62.404543535822555</v>
       </c>
-      <c r="N6">
+      <c r="O6">
         <f t="shared" si="3"/>
         <v>1.4377630249306061</v>
       </c>
-      <c r="O6">
+      <c r="P6">
         <f t="shared" si="4"/>
         <v>0.2148969645803753</v>
       </c>
-      <c r="P6">
+      <c r="Q6">
         <f t="shared" si="5"/>
         <v>1.6526599895109815</v>
       </c>
-      <c r="Q6">
+      <c r="R6">
         <f t="shared" si="6"/>
         <v>5.9902528876779622</v>
       </c>
-      <c r="R6">
+      <c r="S6">
         <f t="shared" si="7"/>
         <v>29.489491794261742</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>171003020502</v>
       </c>
@@ -2185,60 +2204,63 @@
         <v>31</v>
       </c>
       <c r="D7">
+        <v>90.75</v>
+      </c>
+      <c r="E7">
         <v>888</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>256</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>1699</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>24574</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>26622</v>
       </c>
-      <c r="I7">
+      <c r="J7">
         <v>87</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <v>17</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <f t="shared" si="0"/>
         <v>54143</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <f t="shared" si="1"/>
         <v>1144</v>
       </c>
-      <c r="M7">
+      <c r="N7">
         <f t="shared" si="2"/>
         <v>49.169791108730578</v>
       </c>
-      <c r="N7">
+      <c r="O7">
         <f t="shared" si="3"/>
         <v>1.6401012134532627</v>
       </c>
-      <c r="O7">
+      <c r="P7">
         <f t="shared" si="4"/>
         <v>0.47282197144598564</v>
       </c>
-      <c r="P7">
+      <c r="Q7">
         <f t="shared" si="5"/>
         <v>2.1129231848992482</v>
       </c>
-      <c r="Q7">
+      <c r="R7">
         <f t="shared" si="6"/>
         <v>3.1379864433075375</v>
       </c>
-      <c r="R7">
+      <c r="S7">
         <f t="shared" si="7"/>
         <v>45.387215337162701</v>
       </c>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>171003020306</v>
       </c>
@@ -2248,61 +2270,61 @@
       <c r="C8" t="s">
         <v>32</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>106</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>18</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>600</v>
       </c>
-      <c r="G8">
+      <c r="H8">
         <v>9755</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>35721</v>
       </c>
-      <c r="I8">
+      <c r="J8">
         <v>76</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <v>30</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <f t="shared" si="0"/>
         <v>46306</v>
       </c>
-      <c r="L8">
+      <c r="M8">
         <f t="shared" si="1"/>
         <v>124</v>
       </c>
-      <c r="M8">
+      <c r="N8">
         <f t="shared" si="2"/>
         <v>77.141191206323157</v>
       </c>
-      <c r="N8">
+      <c r="O8">
         <f t="shared" si="3"/>
         <v>0.22891202004059946</v>
       </c>
-      <c r="O8">
+      <c r="P8">
         <f t="shared" si="4"/>
         <v>3.8871852459724444E-2</v>
       </c>
-      <c r="P8">
+      <c r="Q8">
         <f t="shared" si="5"/>
         <v>0.26778387250032393</v>
       </c>
-      <c r="Q8">
+      <c r="R8">
         <f t="shared" si="6"/>
         <v>1.295728415324148</v>
       </c>
-      <c r="R8">
+      <c r="S8">
         <f t="shared" si="7"/>
         <v>21.066384485811774</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>171003020903</v>
       </c>
@@ -2313,60 +2335,63 @@
         <v>33</v>
       </c>
       <c r="D9">
+        <v>86.9</v>
+      </c>
+      <c r="E9">
         <v>1945</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>138</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>166</v>
       </c>
-      <c r="G9">
+      <c r="H9">
         <v>15467</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>34100</v>
       </c>
-      <c r="I9">
+      <c r="J9">
         <v>2</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <v>177</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <f t="shared" si="0"/>
         <v>51995</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <f t="shared" si="1"/>
         <v>2083</v>
       </c>
-      <c r="M9">
+      <c r="N9">
         <f t="shared" si="2"/>
         <v>65.583229156649679</v>
       </c>
-      <c r="N9">
+      <c r="O9">
         <f t="shared" si="3"/>
         <v>3.7407443023367635</v>
       </c>
-      <c r="O9">
+      <c r="P9">
         <f t="shared" si="4"/>
         <v>0.26541013558996057</v>
       </c>
-      <c r="P9">
+      <c r="Q9">
         <f t="shared" si="5"/>
         <v>4.0061544379267238</v>
       </c>
-      <c r="Q9">
+      <c r="R9">
         <f t="shared" si="6"/>
         <v>0.31926146744879313</v>
       </c>
-      <c r="R9">
+      <c r="S9">
         <f t="shared" si="7"/>
         <v>29.747091066448693</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>171003020902</v>
       </c>
@@ -2377,60 +2402,63 @@
         <v>16</v>
       </c>
       <c r="D10">
+        <v>133.66</v>
+      </c>
+      <c r="E10">
         <v>2780</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>266</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>0</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>37797</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>38818</v>
       </c>
-      <c r="I10">
+      <c r="J10">
         <v>1</v>
       </c>
-      <c r="J10">
+      <c r="K10">
         <v>173</v>
       </c>
-      <c r="K10">
+      <c r="L10">
         <f t="shared" si="0"/>
         <v>79835</v>
       </c>
-      <c r="L10">
+      <c r="M10">
         <f t="shared" si="1"/>
         <v>3046</v>
       </c>
-      <c r="M10">
+      <c r="N10">
         <f t="shared" si="2"/>
         <v>48.622784493016844</v>
       </c>
-      <c r="N10">
+      <c r="O10">
         <f t="shared" si="3"/>
         <v>3.4821820003757749</v>
       </c>
-      <c r="O10">
+      <c r="P10">
         <f t="shared" si="4"/>
         <v>0.33318719859710655</v>
       </c>
-      <c r="P10">
+      <c r="Q10">
         <f t="shared" si="5"/>
         <v>3.8153691989728817</v>
       </c>
-      <c r="Q10">
+      <c r="R10">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="R10">
+      <c r="S10">
         <f t="shared" si="7"/>
         <v>47.343896787123441</v>
       </c>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>171003020303</v>
       </c>
@@ -2440,9 +2468,6 @@
       <c r="C11" t="s">
         <v>45</v>
       </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
       <c r="E11">
         <v>0</v>
       </c>
@@ -2450,46 +2475,49 @@
         <v>0</v>
       </c>
       <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
         <v>10125</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>53397</v>
       </c>
-      <c r="I11">
+      <c r="J11">
         <v>0</v>
       </c>
-      <c r="J11">
+      <c r="K11">
         <v>3</v>
       </c>
-      <c r="K11">
+      <c r="L11">
         <f t="shared" si="0"/>
         <v>63525</v>
       </c>
-      <c r="L11">
+      <c r="M11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M11">
+      <c r="N11">
         <f t="shared" si="2"/>
         <v>84.056670602125152</v>
       </c>
-      <c r="N11">
+      <c r="O11">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="O11">
+      <c r="P11">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="P11">
+      <c r="Q11">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="Q11">
+      <c r="R11">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="R11">
+      <c r="S11">
         <f t="shared" si="7"/>
         <v>15.938606847697756</v>
       </c>

</xml_diff>